<commit_message>
today's entry + data
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/O6_crizotinib_selumetinib_ABT/Crizotinib_selumetinib_ABT_SRB_data.xlsx
+++ b/Raw_SRB_data/O6_crizotinib_selumetinib_ABT/Crizotinib_selumetinib_ABT_SRB_data.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CxAxS 1" sheetId="1" r:id="rId1"/>
     <sheet name="CxAxS 2" sheetId="2" r:id="rId2"/>
+    <sheet name="CxAxS 3" sheetId="3" r:id="rId3"/>
+    <sheet name="CxAxS 4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>Crizotinib + Selumetinib + ABT-737</t>
   </si>
@@ -67,6 +69,21 @@
   </si>
   <si>
     <t>ABT and triple combination</t>
+  </si>
+  <si>
+    <t>Replicate # 3</t>
+  </si>
+  <si>
+    <t>Replicate # 4</t>
+  </si>
+  <si>
+    <t>Passage #10</t>
+  </si>
+  <si>
+    <t>Day  1 date: 21/10/19</t>
+  </si>
+  <si>
+    <t>Day  1 date: 24/10/19</t>
   </si>
 </sst>
 </file>
@@ -164,8 +181,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FFCCCCFF"/>
-      <color rgb="FFFFCCFF"/>
       <color rgb="FFFFABFF"/>
       <color rgb="FFFF99FF"/>
     </mruColors>
@@ -1469,7 +1486,1029 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="B8">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C8">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="D8">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F8">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G8">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="H8">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="I8">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="J8">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="K8">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="L8">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="N8">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="O8">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="P8">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="Q8">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="R8">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="S8">
+        <v>6.2E-2</v>
+      </c>
+      <c r="T8">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="U8">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="V8">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="W8">
+        <v>0.126</v>
+      </c>
+      <c r="X8">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="Y8">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.429</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.2669999999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.208</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.0509999999999999</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="I9">
+        <v>0.15</v>
+      </c>
+      <c r="J9">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="K9">
+        <v>0.127</v>
+      </c>
+      <c r="L9">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="N9">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="O9" s="4">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="P9" s="4">
+        <v>1.282</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>1.256</v>
+      </c>
+      <c r="R9" s="4">
+        <v>1.016</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="T9" s="4">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="U9" s="4">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="V9">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="W9">
+        <v>0.11</v>
+      </c>
+      <c r="X9">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="Y9">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.131</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="I10">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="J10">
+        <v>0.108</v>
+      </c>
+      <c r="K10">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="L10">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="N10">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="O10" s="4">
+        <v>1.391</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>1.615</v>
+      </c>
+      <c r="R10" s="4">
+        <v>1.054</v>
+      </c>
+      <c r="S10" s="4">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="T10" s="4">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="U10" s="4">
+        <v>0.18</v>
+      </c>
+      <c r="V10">
+        <v>0.08</v>
+      </c>
+      <c r="W10">
+        <v>0.09</v>
+      </c>
+      <c r="X10">
+        <v>0.106</v>
+      </c>
+      <c r="Y10">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="I11">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="J11">
+        <v>0.12</v>
+      </c>
+      <c r="K11">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="L11">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="N11">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="O11" s="4">
+        <v>1.242</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1.2989999999999999</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="R11" s="4">
+        <v>1.151</v>
+      </c>
+      <c r="S11" s="4">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="T11" s="4">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="U11" s="4">
+        <v>0.188</v>
+      </c>
+      <c r="V11">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="W11">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="X11">
+        <v>0.105</v>
+      </c>
+      <c r="Y11">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.186</v>
+      </c>
+      <c r="I12">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="J12">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="K12">
+        <v>0.122</v>
+      </c>
+      <c r="L12">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="N12">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="O12" s="5">
+        <v>1.121</v>
+      </c>
+      <c r="P12" s="5">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="S12" s="5">
+        <v>0.193</v>
+      </c>
+      <c r="T12" s="5">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="U12" s="5">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="V12">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="W12">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="X12">
+        <v>0.12</v>
+      </c>
+      <c r="Y12">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7.8E-2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.182</v>
+      </c>
+      <c r="I13">
+        <v>0.107</v>
+      </c>
+      <c r="J13">
+        <v>0.12</v>
+      </c>
+      <c r="K13">
+        <v>0.112</v>
+      </c>
+      <c r="L13">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="N13">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="P13" s="5">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>0.437</v>
+      </c>
+      <c r="R13" s="5">
+        <v>0.376</v>
+      </c>
+      <c r="S13" s="5">
+        <v>0.191</v>
+      </c>
+      <c r="T13" s="5">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="U13" s="5">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="V13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W13">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="X13">
+        <v>0.121</v>
+      </c>
+      <c r="Y13">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.216</v>
+      </c>
+      <c r="I14">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="J14">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="K14">
+        <v>0.126</v>
+      </c>
+      <c r="L14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="N14">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="O14" s="5">
+        <v>1.603</v>
+      </c>
+      <c r="P14" s="5">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>0.438</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0.185</v>
+      </c>
+      <c r="T14" s="5">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="U14" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="V14">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="W14">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="X14">
+        <v>0.112</v>
+      </c>
+      <c r="Y14">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="B15">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="C15">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D15">
+        <v>9.4E-2</v>
+      </c>
+      <c r="E15">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F15">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="G15">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="H15">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="I15">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="J15">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="K15">
+        <v>9.4E-2</v>
+      </c>
+      <c r="L15">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="N15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="O15">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="P15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q15">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="R15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="S15">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="T15">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="U15">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="V15">
+        <v>7.8E-2</v>
+      </c>
+      <c r="W15">
+        <v>0.08</v>
+      </c>
+      <c r="X15">
+        <v>0.115</v>
+      </c>
+      <c r="Y15">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <f>AVERAGE(B9:B11)</f>
+        <v>1.1453333333333333</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:H17" si="0">AVERAGE(C9:C11)</f>
+        <v>1.0860000000000001</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1.0263333333333333</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.9986666666666667</v>
+      </c>
+      <c r="F17">
+        <f>AVERAGE(F9:F11)</f>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0.6156666666666667</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17">
+        <f>AVERAGE(O9:O11)</f>
+        <v>1.2873333333333334</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ref="P17:U17" si="1">AVERAGE(P9:P11)</f>
+        <v>1.3453333333333333</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="1"/>
+        <v>1.647</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>1.0736666666666668</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="1"/>
+        <v>0.97333333333333327</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>0.44666666666666671</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="1"/>
+        <v>0.16866666666666666</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <f>AVERAGE(B12:B14)</f>
+        <v>1.0190000000000001</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:G19" si="2">AVERAGE(C12:C14)</f>
+        <v>0.6216666666666667</v>
+      </c>
+      <c r="D19">
+        <f>AVERAGE(D12:D14)</f>
+        <v>0.45599999999999996</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0.52433333333333343</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>0.59433333333333327</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>0.41233333333333338</v>
+      </c>
+      <c r="H19">
+        <f>AVERAGE(H12:H14)</f>
+        <v>0.19466666666666665</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19">
+        <f>AVERAGE(O12:O14)</f>
+        <v>1.3336666666666666</v>
+      </c>
+      <c r="P19">
+        <f t="shared" ref="P19:U19" si="3">AVERAGE(P12:P14)</f>
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="Q19">
+        <f>AVERAGE(Q12:Q14)</f>
+        <v>0.47366666666666668</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="3"/>
+        <v>0.40966666666666668</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="3"/>
+        <v>0.18966666666666665</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="3"/>
+        <v>0.13966666666666669</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="3"/>
+        <v>0.12466666666666666</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1.1453333333333333</v>
+      </c>
+      <c r="D22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>1.0190000000000001</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+      <c r="I22">
+        <v>1.2873333333333334</v>
+      </c>
+      <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="L22">
+        <v>1.3336666666666666</v>
+      </c>
+      <c r="M22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.1</v>
+      </c>
+      <c r="C23">
+        <v>1.0860000000000001</v>
+      </c>
+      <c r="D23">
+        <f>C23/1.145333*100</f>
+        <v>94.819585221066731</v>
+      </c>
+      <c r="F23">
+        <v>0.6216666666666667</v>
+      </c>
+      <c r="G23">
+        <f>F23/1.019*100</f>
+        <v>61.007523716061506</v>
+      </c>
+      <c r="I23">
+        <v>1.3453333333333333</v>
+      </c>
+      <c r="J23">
+        <f>I23/1.287333*100</f>
+        <v>104.50546465703383</v>
+      </c>
+      <c r="L23">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="M23">
+        <f>L23/1.333667*100</f>
+        <v>49.187690780382212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.2</v>
+      </c>
+      <c r="C24">
+        <v>1.0263333333333333</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ref="D24:D28" si="4">C24/1.145333*100</f>
+        <v>89.61003772119841</v>
+      </c>
+      <c r="F24">
+        <v>0.45599999999999996</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24:G28" si="5">F24/1.019*100</f>
+        <v>44.749754661432775</v>
+      </c>
+      <c r="I24">
+        <v>1.647</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ref="J24:J28" si="6">I24/1.287333*100</f>
+        <v>127.938924893559</v>
+      </c>
+      <c r="L24">
+        <v>0.47366666666666668</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:M28" si="7">L24/1.333667*100</f>
+        <v>35.516112092948745</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.3</v>
+      </c>
+      <c r="C25">
+        <v>0.9986666666666667</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="4"/>
+        <v>87.194437483829319</v>
+      </c>
+      <c r="F25">
+        <v>0.52433333333333343</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>51.455675498855101</v>
+      </c>
+      <c r="I25">
+        <v>1.0736666666666668</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="6"/>
+        <v>83.40240378104707</v>
+      </c>
+      <c r="L25">
+        <v>0.40966666666666668</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="7"/>
+        <v>30.717312992423651</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.5</v>
+      </c>
+      <c r="C26">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="4"/>
+        <v>79.889429537086599</v>
+      </c>
+      <c r="F26">
+        <v>0.59433333333333327</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>58.325155381092571</v>
+      </c>
+      <c r="I26">
+        <v>0.97333333333333327</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="6"/>
+        <v>75.608512586357463</v>
+      </c>
+      <c r="L26">
+        <v>0.18966666666666665</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="7"/>
+        <v>14.221441084368635</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0.6156666666666667</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="4"/>
+        <v>53.754381185791964</v>
+      </c>
+      <c r="F27">
+        <v>0.41233333333333338</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>40.464507687275116</v>
+      </c>
+      <c r="I27">
+        <v>0.44666666666666671</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="6"/>
+        <v>34.697057145794183</v>
+      </c>
+      <c r="L27">
+        <v>0.13966666666666669</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="7"/>
+        <v>10.47237928708341</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="4"/>
+        <v>24.097795139055631</v>
+      </c>
+      <c r="F28">
+        <v>0.19466666666666665</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>19.103696434412822</v>
+      </c>
+      <c r="I28">
+        <v>0.16866666666666666</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="6"/>
+        <v>13.102023071471535</v>
+      </c>
+      <c r="L28">
+        <v>0.12466666666666666</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="7"/>
+        <v>9.3476607478978391</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="M22" sqref="M22:M28"/>
     </sheetView>
   </sheetViews>
@@ -1485,7 +2524,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1493,7 +2532,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1501,7 +2540,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1526,52 +2565,1075 @@
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="B8">
-        <v>6.6000000000000003E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="C8">
-        <v>6.4000000000000001E-2</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="D8">
-        <v>6.4000000000000001E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="E8">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="F8">
-        <v>7.5999999999999998E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G8">
-        <v>7.1999999999999995E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="H8">
-        <v>9.7000000000000003E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="I8">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="J8">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="K8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L8">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="N8">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="O8">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="P8">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="Q8">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="R8">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="S8">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="T8">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="U8">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="V8">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="W8">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="X8">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="Y8">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.6739999999999999</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.694</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.4319999999999999</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.9890000000000001</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.0740000000000001</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.311</v>
+      </c>
+      <c r="I9">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J9">
+        <v>5.5E-2</v>
+      </c>
+      <c r="K9">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="L9">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="N9">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="O9" s="4">
+        <v>1.5860000000000001</v>
+      </c>
+      <c r="P9" s="4">
+        <v>1.917</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>2.056</v>
+      </c>
+      <c r="R9" s="4">
+        <v>1.3859999999999999</v>
+      </c>
+      <c r="S9" s="4">
+        <v>1.714</v>
+      </c>
+      <c r="T9" s="4">
+        <v>1.143</v>
+      </c>
+      <c r="U9" s="4">
+        <v>1.355</v>
+      </c>
+      <c r="V9">
+        <v>0.111</v>
+      </c>
+      <c r="W9">
+        <v>9.4E-2</v>
+      </c>
+      <c r="X9">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="Y9">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.391</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.258</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.1219999999999999</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.754</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.76400000000000001</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="I10">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="J10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="K10">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L10">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="N10">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="O10" s="4">
+        <v>1.7529999999999999</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1.611</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>1.76</v>
+      </c>
+      <c r="R10" s="4">
+        <v>1.262</v>
+      </c>
+      <c r="S10" s="4">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="T10" s="4">
+        <v>1.0549999999999999</v>
+      </c>
+      <c r="U10" s="4">
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="V10">
+        <v>0.112</v>
+      </c>
+      <c r="W10">
+        <v>0.105</v>
+      </c>
+      <c r="X10">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="Y10">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.929</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1.6579999999999999</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.054</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.9179999999999999</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.605</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="I11">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="J11">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="K11">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="L11">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="N11">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O11" s="4">
+        <v>1.867</v>
+      </c>
+      <c r="P11" s="4">
+        <v>1.8169999999999999</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>1.7689999999999999</v>
+      </c>
+      <c r="R11" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="S11" s="4">
+        <v>1.196</v>
+      </c>
+      <c r="T11" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="U11" s="4">
+        <v>1.1779999999999999</v>
+      </c>
+      <c r="V11">
+        <v>0.111</v>
+      </c>
+      <c r="W11">
+        <v>0.125</v>
+      </c>
+      <c r="X11">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="Y11">
         <v>6.9000000000000006E-2</v>
       </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2.371</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.372</v>
+      </c>
+      <c r="I12">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="J12">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="K12">
+        <v>4.7E-2</v>
+      </c>
+      <c r="L12">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N12">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="O12" s="5">
+        <v>1.54</v>
+      </c>
+      <c r="P12" s="5">
+        <v>1.018</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="S12" s="5">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="T12" s="5">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="U12" s="5">
+        <v>0.185</v>
+      </c>
+      <c r="V12">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="W12">
+        <v>0.13</v>
+      </c>
+      <c r="X12">
+        <v>0.11</v>
+      </c>
+      <c r="Y12">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2.089</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="I13">
+        <v>6.2E-2</v>
+      </c>
+      <c r="J13">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="K13">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="L13">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="N13">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1.5840000000000001</v>
+      </c>
+      <c r="P13" s="5">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="R13" s="5">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="S13" s="5">
+        <v>0.434</v>
+      </c>
+      <c r="T13" s="5">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="U13" s="5">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="V13">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="W13">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="X13">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="Y13">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.927</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="I14">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="J14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K14">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L14">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="N14">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="O14" s="5">
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="P14" s="5">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="T14" s="5">
+        <v>0.249</v>
+      </c>
+      <c r="U14" s="5">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="V14">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="W14">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="X14">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="Y14">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.05</v>
+      </c>
+      <c r="B15">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C15">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="D15">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E15">
+        <v>0.05</v>
+      </c>
+      <c r="F15">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="G15">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="H15">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="I15">
+        <v>4.7E-2</v>
+      </c>
+      <c r="J15">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K15">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="L15">
+        <v>0.104</v>
+      </c>
+      <c r="N15">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="O15">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="P15">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="Q15">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="R15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S15">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="T15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U15">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="V15">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="W15">
+        <v>0.08</v>
+      </c>
+      <c r="X15">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="Y15">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <f>AVERAGE(B9:B11)</f>
+        <v>1.6646666666666665</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:H17" si="0">AVERAGE(C9:C11)</f>
+        <v>1.5366666666666664</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1.5359999999999998</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1.8870000000000002</v>
+      </c>
+      <c r="F17">
+        <f>AVERAGE(F9:F11)</f>
+        <v>1.248</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>0.81166666666666665</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.36400000000000005</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17">
+        <f>AVERAGE(O9:O11)</f>
+        <v>1.7353333333333332</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ref="P17:U17" si="1">AVERAGE(P9:P11)</f>
+        <v>1.7816666666666665</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="1"/>
+        <v>1.8616666666666666</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>1.2326666666666666</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="1"/>
+        <v>1.4953333333333332</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>1.0493333333333332</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="1"/>
+        <v>1.2050000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <f>AVERAGE(B12:B14)</f>
+        <v>2.129</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:G19" si="2">AVERAGE(C12:C14)</f>
+        <v>0.84166666666666667</v>
+      </c>
+      <c r="D19">
+        <f>AVERAGE(D12:D14)</f>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0.68633333333333335</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>0.77099999999999991</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>0.59333333333333327</v>
+      </c>
+      <c r="H19">
+        <f>AVERAGE(H12:H14)</f>
+        <v>0.35266666666666668</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19">
+        <f>AVERAGE(O12:O14)</f>
+        <v>1.5263333333333335</v>
+      </c>
+      <c r="P19">
+        <f t="shared" ref="P19:U19" si="3">AVERAGE(P12:P14)</f>
+        <v>0.90033333333333332</v>
+      </c>
+      <c r="Q19">
+        <f>AVERAGE(Q12:Q14)</f>
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="3"/>
+        <v>0.48466666666666675</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="3"/>
+        <v>0.40700000000000003</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="3"/>
+        <v>0.26</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="3"/>
+        <v>0.16833333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1.6646666666666665</v>
+      </c>
+      <c r="D22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>2.129</v>
+      </c>
+      <c r="G22">
+        <v>100</v>
+      </c>
+      <c r="I22">
+        <v>1.7353333333333332</v>
+      </c>
+      <c r="J22">
+        <v>100</v>
+      </c>
+      <c r="L22">
+        <v>1.5263333333333335</v>
+      </c>
+      <c r="M22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.1</v>
+      </c>
+      <c r="C23">
+        <v>1.5366666666666664</v>
+      </c>
+      <c r="D23">
+        <f>C23/1.664667*100</f>
+        <v>92.310754443180926</v>
+      </c>
+      <c r="F23">
+        <v>0.84166666666666667</v>
+      </c>
+      <c r="G23">
+        <f>F23/2.129*100</f>
+        <v>39.533427274150618</v>
+      </c>
+      <c r="I23">
+        <v>1.7816666666666665</v>
+      </c>
+      <c r="J23">
+        <f>I23/1.735333*100</f>
+        <v>102.67001587975717</v>
+      </c>
+      <c r="L23">
+        <v>0.90033333333333332</v>
+      </c>
+      <c r="M23">
+        <f>L23/1.526333*100</f>
+        <v>58.98669119604525</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.2</v>
+      </c>
+      <c r="C24">
+        <v>1.5359999999999998</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ref="D24:D28" si="4">C24/1.664667*100</f>
+        <v>92.270706393530958</v>
+      </c>
+      <c r="F24">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24:G28" si="5">F24/2.129*100</f>
+        <v>33.27070612180993</v>
+      </c>
+      <c r="I24">
+        <v>1.8616666666666666</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ref="J24:J28" si="6">I24/1.735333*100</f>
+        <v>107.28008207454516</v>
+      </c>
+      <c r="L24">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:M28" si="7">L24/1.526333*100</f>
+        <v>47.892563418336628</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.3</v>
+      </c>
+      <c r="C25">
+        <v>1.8870000000000002</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="4"/>
+        <v>113.3560045342402</v>
+      </c>
+      <c r="F25">
+        <v>0.68633333333333335</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>32.237357131673711</v>
+      </c>
+      <c r="I25">
+        <v>1.2326666666666666</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="6"/>
+        <v>71.033436618024709</v>
+      </c>
+      <c r="L25">
+        <v>0.48466666666666675</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="7"/>
+        <v>31.753664938559723</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.5</v>
+      </c>
+      <c r="C26">
+        <v>1.248</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="4"/>
+        <v>74.969948944743919</v>
+      </c>
+      <c r="F26">
+        <v>0.77099999999999991</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>36.214185063410049</v>
+      </c>
+      <c r="I26">
+        <v>1.4953333333333332</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="6"/>
+        <v>86.169820624245204</v>
+      </c>
+      <c r="L26">
+        <v>0.40700000000000003</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="7"/>
+        <v>26.665216568075252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0.81166666666666665</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="4"/>
+        <v>48.758500448838518</v>
+      </c>
+      <c r="F27">
+        <v>0.59333333333333327</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>27.869109127916076</v>
+      </c>
+      <c r="I27">
+        <v>1.0493333333333332</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="6"/>
+        <v>60.468701588302253</v>
+      </c>
+      <c r="L27">
+        <v>0.26</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="7"/>
+        <v>17.034290682308516</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>0.36400000000000005</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="4"/>
+        <v>21.866235108883643</v>
+      </c>
+      <c r="F28">
+        <v>0.35266666666666668</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>16.564897447941132</v>
+      </c>
+      <c r="I28">
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="6"/>
+        <v>69.43912205899386</v>
+      </c>
+      <c r="L28">
+        <v>0.16833333333333333</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="7"/>
+        <v>11.028611275084359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.06</v>
+      </c>
+      <c r="B8">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C8">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="D8">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.06</v>
+      </c>
+      <c r="F8">
+        <v>6.2E-2</v>
+      </c>
+      <c r="G8">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H8">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="I8">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="J8">
-        <v>9.8000000000000004E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="K8">
-        <v>9.0999999999999998E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="L8">
-        <v>8.5999999999999993E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="N8">
-        <v>7.3999999999999996E-2</v>
+        <v>0.06</v>
       </c>
       <c r="O8">
-        <v>6.5000000000000002E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="P8">
-        <v>6.7000000000000004E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="Q8">
-        <v>6.5000000000000002E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="R8">
-        <v>6.9000000000000006E-2</v>
+        <v>0.06</v>
       </c>
       <c r="S8">
         <v>6.2E-2</v>
@@ -1580,315 +3642,315 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="U8">
-        <v>6.8000000000000005E-2</v>
+        <v>0.06</v>
       </c>
       <c r="V8">
-        <v>6.9000000000000006E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="W8">
-        <v>0.126</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="X8">
-        <v>0.10199999999999999</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="Y8">
-        <v>9.4E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6.5000000000000002E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="B9" s="2">
-        <v>1.429</v>
+        <v>1.4770000000000001</v>
       </c>
       <c r="C9" s="2">
-        <v>1.2669999999999999</v>
+        <v>0.67300000000000004</v>
       </c>
       <c r="D9" s="2">
-        <v>1.208</v>
+        <v>1.51</v>
       </c>
       <c r="E9" s="2">
-        <v>1.0509999999999999</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="F9" s="2">
-        <v>0.94099999999999995</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="G9" s="2">
-        <v>0.72899999999999998</v>
+        <v>0.625</v>
       </c>
       <c r="H9" s="2">
-        <v>0.26700000000000002</v>
+        <v>0.245</v>
       </c>
       <c r="I9">
-        <v>0.15</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="J9">
-        <v>9.7000000000000003E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="K9">
-        <v>0.127</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="L9">
-        <v>8.1000000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="N9">
-        <v>6.7000000000000004E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="O9" s="4">
-        <v>1.2290000000000001</v>
+        <v>1.2390000000000001</v>
       </c>
       <c r="P9" s="4">
-        <v>1.282</v>
+        <v>0.622</v>
       </c>
       <c r="Q9" s="4">
-        <v>1.256</v>
+        <v>1.321</v>
       </c>
       <c r="R9" s="4">
-        <v>1.016</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="S9" s="4">
-        <v>0.96299999999999997</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="T9" s="4">
-        <v>0.45200000000000001</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="U9" s="4">
-        <v>0.13800000000000001</v>
+        <v>0.28899999999999998</v>
       </c>
       <c r="V9">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="W9">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="X9">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="W9">
-        <v>0.11</v>
-      </c>
-      <c r="X9">
-        <v>0.10199999999999999</v>
-      </c>
       <c r="Y9">
-        <v>0.104</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7.4999999999999997E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="B10" s="2">
-        <v>1.1679999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="C10" s="2">
-        <v>1.01</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="D10" s="2">
-        <v>1.131</v>
+        <v>1.2350000000000001</v>
       </c>
       <c r="E10" s="2">
-        <v>0.93200000000000005</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="F10" s="2">
-        <v>0.82899999999999996</v>
+        <v>1.1759999999999999</v>
       </c>
       <c r="G10" s="2">
-        <v>0.56899999999999995</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="H10" s="2">
-        <v>0.27900000000000003</v>
+        <v>0.253</v>
       </c>
       <c r="I10">
-        <v>0.10100000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="J10">
-        <v>0.108</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="K10">
-        <v>0.11700000000000001</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="L10">
-        <v>9.8000000000000004E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="N10">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="O10" s="4">
-        <v>1.391</v>
+        <v>1.198</v>
       </c>
       <c r="P10" s="4">
-        <v>1.4550000000000001</v>
+        <v>0.56699999999999995</v>
       </c>
       <c r="Q10" s="4">
-        <v>1.615</v>
+        <v>1.1950000000000001</v>
       </c>
       <c r="R10" s="4">
-        <v>1.054</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="S10" s="4">
-        <v>1.0009999999999999</v>
+        <v>1.143</v>
       </c>
       <c r="T10" s="4">
-        <v>0.42399999999999999</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="U10" s="4">
-        <v>0.18</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="V10">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="W10">
-        <v>0.09</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="X10">
-        <v>0.106</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="Y10">
-        <v>0.104</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6.7000000000000004E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="B11" s="2">
-        <v>0.83899999999999997</v>
+        <v>1.109</v>
       </c>
       <c r="C11" s="2">
-        <v>0.98099999999999998</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="D11" s="2">
-        <v>0.74</v>
+        <v>0.88400000000000001</v>
       </c>
       <c r="E11" s="2">
-        <v>1.0129999999999999</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="F11" s="2">
-        <v>0.97499999999999998</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="G11" s="2">
-        <v>0.54900000000000004</v>
+        <v>0.39800000000000002</v>
       </c>
       <c r="H11" s="2">
-        <v>0.28199999999999997</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="I11">
-        <v>0.11700000000000001</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="J11">
-        <v>0.12</v>
+        <v>6.2E-2</v>
       </c>
       <c r="K11">
-        <v>9.5000000000000001E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="L11">
-        <v>9.6000000000000002E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="N11">
-        <v>6.7000000000000004E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="O11" s="4">
-        <v>1.242</v>
+        <v>1.153</v>
       </c>
       <c r="P11" s="4">
-        <v>1.2989999999999999</v>
+        <v>0.624</v>
       </c>
       <c r="Q11" s="4">
-        <v>2.0699999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="R11" s="4">
-        <v>1.151</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="S11" s="4">
-        <v>0.95599999999999996</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="T11" s="4">
-        <v>0.46400000000000002</v>
+        <v>0.439</v>
       </c>
       <c r="U11" s="4">
-        <v>0.188</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="V11">
-        <v>7.0999999999999994E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="W11">
-        <v>6.8000000000000005E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="X11">
-        <v>0.105</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="Y11">
-        <v>0.111</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>6.9000000000000006E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="B12" s="3">
-        <v>0.96299999999999997</v>
+        <v>1.3</v>
       </c>
       <c r="C12" s="3">
-        <v>0.75700000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="D12" s="3">
-        <v>0.42099999999999999</v>
+        <v>0.52</v>
       </c>
       <c r="E12" s="3">
-        <v>0.51800000000000002</v>
+        <v>0.47099999999999997</v>
       </c>
       <c r="F12" s="3">
-        <v>0.52800000000000002</v>
+        <v>0.374</v>
       </c>
       <c r="G12" s="3">
-        <v>0.51900000000000002</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="H12" s="3">
-        <v>0.186</v>
+        <v>0.218</v>
       </c>
       <c r="I12">
-        <v>0.11700000000000001</v>
+        <v>6.2E-2</v>
       </c>
       <c r="J12">
-        <v>9.0999999999999998E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="K12">
-        <v>0.122</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L12">
-        <v>8.8999999999999996E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="N12">
-        <v>6.5000000000000002E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="O12" s="5">
-        <v>1.121</v>
+        <v>1.2949999999999999</v>
       </c>
       <c r="P12" s="5">
-        <v>0.50700000000000001</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="Q12" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="R12" s="5">
         <v>0.54600000000000004</v>
       </c>
-      <c r="R12" s="5">
-        <v>0.29899999999999999</v>
-      </c>
       <c r="S12" s="5">
-        <v>0.193</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="T12" s="5">
-        <v>0.14599999999999999</v>
+        <v>0.443</v>
       </c>
       <c r="U12" s="5">
-        <v>0.11700000000000001</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="V12">
-        <v>7.5999999999999998E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="W12">
-        <v>7.6999999999999999E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="X12">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="Y12">
-        <v>0.107</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -1896,221 +3958,221 @@
         <v>7.8E-2</v>
       </c>
       <c r="B13" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.2529999999999999</v>
       </c>
       <c r="C13" s="3">
-        <v>0.56000000000000005</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="D13" s="3">
-        <v>0.46800000000000003</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="E13" s="3">
-        <v>0.54100000000000004</v>
+        <v>0.504</v>
       </c>
       <c r="F13" s="3">
-        <v>0.70199999999999996</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="G13" s="3">
-        <v>0.38600000000000001</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="H13" s="3">
-        <v>0.182</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="I13">
-        <v>0.107</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="J13">
-        <v>0.12</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="K13">
-        <v>0.112</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="L13">
-        <v>8.6999999999999994E-2</v>
+        <v>0.06</v>
       </c>
       <c r="N13">
-        <v>8.4000000000000005E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="O13" s="5">
-        <v>1.2769999999999999</v>
+        <v>1.218</v>
       </c>
       <c r="P13" s="5">
-        <v>0.60799999999999998</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="Q13" s="5">
-        <v>0.437</v>
+        <v>0.66</v>
       </c>
       <c r="R13" s="5">
-        <v>0.376</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="S13" s="5">
-        <v>0.191</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="T13" s="5">
-        <v>0.13600000000000001</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="U13" s="5">
-        <v>0.11700000000000001</v>
+        <v>0.253</v>
       </c>
       <c r="V13">
-        <v>7.0000000000000007E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="W13">
-        <v>6.5000000000000002E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="X13">
-        <v>0.121</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="Y13">
-        <v>9.4E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.1439999999999999</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="I14">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="J14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K14">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="L14">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="B14" s="3">
-        <v>0.99399999999999999</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.55300000000000005</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.33200000000000002</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0.216</v>
-      </c>
-      <c r="I14">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="J14">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="K14">
-        <v>0.126</v>
-      </c>
-      <c r="L14">
+      <c r="N14">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="O14" s="5">
+        <v>1.097</v>
+      </c>
+      <c r="P14" s="5">
+        <v>0.747</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0.437</v>
+      </c>
+      <c r="T14" s="5">
+        <v>0.37</v>
+      </c>
+      <c r="U14" s="5">
+        <v>0.309</v>
+      </c>
+      <c r="V14">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="W14">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X14">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="N14">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="O14" s="5">
-        <v>1.603</v>
-      </c>
-      <c r="P14" s="5">
-        <v>0.85299999999999998</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>0.438</v>
-      </c>
-      <c r="R14" s="5">
-        <v>0.55400000000000005</v>
-      </c>
-      <c r="S14" s="5">
-        <v>0.185</v>
-      </c>
-      <c r="T14" s="5">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="U14" s="5">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="V14">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="W14">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="X14">
-        <v>0.112</v>
-      </c>
       <c r="Y14">
-        <v>0.107</v>
+        <v>6.6000000000000003E-2</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>6.8000000000000005E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="B15">
-        <v>9.7000000000000003E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="C15">
-        <v>6.7000000000000004E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="D15">
-        <v>9.4E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E15">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="F15">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="G15">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="H15">
+        <v>0.08</v>
+      </c>
+      <c r="I15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J15">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="K15">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="L15">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="N15">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="O15">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="P15">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Q15">
+        <v>0.08</v>
+      </c>
+      <c r="R15">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="S15">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="T15">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="U15">
+        <v>0.08</v>
+      </c>
+      <c r="V15">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="W15">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="X15">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="F15">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="G15">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="H15">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="I15">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="J15">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="K15">
-        <v>9.4E-2</v>
-      </c>
-      <c r="L15">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="N15">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="O15">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="P15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q15">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="R15">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="S15">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="T15">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="U15">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="V15">
-        <v>7.8E-2</v>
-      </c>
-      <c r="W15">
-        <v>0.08</v>
-      </c>
-      <c r="X15">
-        <v>0.115</v>
-      </c>
       <c r="Y15">
-        <v>9.4E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -2119,62 +4181,62 @@
       </c>
       <c r="B17">
         <f>AVERAGE(B9:B11)</f>
-        <v>1.1453333333333333</v>
+        <v>1.2786666666666668</v>
       </c>
       <c r="C17">
         <f t="shared" ref="C17:H17" si="0">AVERAGE(C9:C11)</f>
-        <v>1.0860000000000001</v>
+        <v>0.64966666666666673</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>1.0263333333333333</v>
+        <v>1.2096666666666667</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>0.9986666666666667</v>
+        <f>AVERAGE(E9:E11)</f>
+        <v>0.83899999999999997</v>
       </c>
       <c r="F17">
         <f>AVERAGE(F9:F11)</f>
-        <v>0.91500000000000004</v>
+        <v>0.90699999999999992</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
-        <v>0.6156666666666667</v>
+        <f>AVERAGE(G9:G11)</f>
+        <v>0.49266666666666675</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>0.27600000000000002</v>
+        <v>0.24133333333333332</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="O17">
         <f>AVERAGE(O9:O11)</f>
-        <v>1.2873333333333334</v>
+        <v>1.1966666666666668</v>
       </c>
       <c r="P17">
         <f t="shared" ref="P17:U17" si="1">AVERAGE(P9:P11)</f>
-        <v>1.3453333333333333</v>
+        <v>0.60433333333333339</v>
       </c>
       <c r="Q17">
         <f t="shared" si="1"/>
-        <v>1.647</v>
+        <v>1.167</v>
       </c>
       <c r="R17">
         <f t="shared" si="1"/>
-        <v>1.0736666666666668</v>
+        <v>0.79</v>
       </c>
       <c r="S17">
         <f t="shared" si="1"/>
-        <v>0.97333333333333327</v>
+        <v>0.87733333333333341</v>
       </c>
       <c r="T17">
         <f t="shared" si="1"/>
-        <v>0.44666666666666671</v>
+        <v>0.5073333333333333</v>
       </c>
       <c r="U17">
         <f t="shared" si="1"/>
-        <v>0.16866666666666666</v>
+        <v>0.27866666666666667</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -2183,62 +4245,62 @@
       </c>
       <c r="B19">
         <f>AVERAGE(B12:B14)</f>
-        <v>1.0190000000000001</v>
+        <v>1.2323333333333333</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:H19" si="2">AVERAGE(C12:C14)</f>
-        <v>0.6216666666666667</v>
+        <f t="shared" ref="C19:G19" si="2">AVERAGE(C12:C14)</f>
+        <v>0.73699999999999999</v>
       </c>
       <c r="D19">
         <f>AVERAGE(D12:D14)</f>
-        <v>0.45599999999999996</v>
+        <v>0.56900000000000006</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>0.52433333333333343</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
-        <v>0.59433333333333327</v>
+        <v>0.44333333333333336</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>0.41233333333333338</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="H19">
         <f>AVERAGE(H12:H14)</f>
-        <v>0.19466666666666665</v>
+        <v>0.23</v>
       </c>
       <c r="N19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="O19">
         <f>AVERAGE(O12:O14)</f>
-        <v>1.3336666666666666</v>
+        <v>1.2033333333333334</v>
       </c>
       <c r="P19">
         <f t="shared" ref="P19:U19" si="3">AVERAGE(P12:P14)</f>
-        <v>0.65600000000000003</v>
+        <v>0.71266666666666667</v>
       </c>
       <c r="Q19">
         <f>AVERAGE(Q12:Q14)</f>
-        <v>0.47366666666666668</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="R19">
         <f t="shared" si="3"/>
-        <v>0.40966666666666668</v>
+        <v>0.57200000000000006</v>
       </c>
       <c r="S19">
         <f t="shared" si="3"/>
-        <v>0.18966666666666665</v>
+        <v>0.49</v>
       </c>
       <c r="T19">
         <f t="shared" si="3"/>
-        <v>0.13966666666666669</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="U19">
         <f t="shared" si="3"/>
-        <v>0.12466666666666666</v>
+        <v>0.27499999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -2256,230 +4318,209 @@
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>0</v>
-      </c>
       <c r="C22">
-        <v>1.1453333333333333</v>
+        <v>1.2786666666666668</v>
       </c>
       <c r="D22">
         <v>100</v>
       </c>
       <c r="F22">
-        <v>1.0190000000000001</v>
+        <v>1.2323333333333333</v>
       </c>
       <c r="G22">
         <v>100</v>
       </c>
       <c r="I22">
-        <v>1.2873333333333334</v>
+        <v>1.1966666666666668</v>
       </c>
       <c r="J22">
         <v>100</v>
       </c>
       <c r="L22">
-        <v>1.3336666666666666</v>
+        <v>1.2033333333333334</v>
       </c>
       <c r="M22">
         <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>0.1</v>
-      </c>
       <c r="C23">
-        <v>1.0860000000000001</v>
+        <v>0.64966666666666673</v>
       </c>
       <c r="D23">
-        <f>C23/1.145333*100</f>
-        <v>94.819585221066731</v>
+        <f>C23/1.278667*100</f>
+        <v>50.808120227288789</v>
       </c>
       <c r="F23">
-        <v>0.6216666666666667</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="G23">
-        <f>F23/1.019*100</f>
-        <v>61.007523716061506</v>
+        <f>F23/1.232333*100</f>
+        <v>59.805263674672346</v>
       </c>
       <c r="I23">
-        <v>1.3453333333333333</v>
+        <v>0.60433333333333339</v>
       </c>
       <c r="J23">
-        <f>I23/1.287333*100</f>
-        <v>104.50546465703383</v>
+        <f>I23/1.196667*100</f>
+        <v>50.50137869042377</v>
       </c>
       <c r="L23">
-        <v>0.65600000000000003</v>
+        <v>0.71266666666666667</v>
       </c>
       <c r="M23">
-        <f>L23/1.333667*100</f>
-        <v>49.187690780382212</v>
+        <f>L23/1.203333*100</f>
+        <v>59.224393136951001</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>0.2</v>
-      </c>
       <c r="C24">
-        <v>1.0263333333333333</v>
+        <v>1.2096666666666667</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D24:D28" si="4">C24/1.145333*100</f>
-        <v>89.61003772119841</v>
+        <f t="shared" ref="D24:D28" si="4">C24/1.278667*100</f>
+        <v>94.603729248245756</v>
       </c>
       <c r="F24">
-        <v>0.45599999999999996</v>
+        <v>0.56900000000000006</v>
       </c>
       <c r="G24">
-        <f t="shared" ref="G24:G28" si="5">F24/1.019*100</f>
-        <v>44.749754661432775</v>
+        <f t="shared" ref="G24:G28" si="5">F24/1.232333*100</f>
+        <v>46.17258484516767</v>
       </c>
       <c r="I24">
-        <v>1.647</v>
+        <v>1.167</v>
       </c>
       <c r="J24">
-        <f t="shared" ref="J24:J28" si="6">I24/1.287333*100</f>
-        <v>127.938924893559</v>
+        <f t="shared" ref="J24:J28" si="6">I24/1.196667*100</f>
+        <v>97.520864200316396</v>
       </c>
       <c r="L24">
-        <v>0.47366666666666668</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="M24">
-        <f t="shared" ref="M24:M28" si="7">L24/1.333667*100</f>
-        <v>35.516112092948745</v>
+        <f t="shared" ref="M24:M28" si="7">L24/1.203333*100</f>
+        <v>50.277022237402278</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>0.3</v>
-      </c>
       <c r="C25">
-        <v>0.9986666666666667</v>
+        <v>0.83899999999999997</v>
       </c>
       <c r="D25">
         <f t="shared" si="4"/>
-        <v>87.194437483829319</v>
+        <v>65.615207086755191</v>
       </c>
       <c r="F25">
-        <v>0.52433333333333343</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="G25">
         <f t="shared" si="5"/>
-        <v>51.455675498855101</v>
+        <v>42.926708933380837</v>
       </c>
       <c r="I25">
-        <v>1.0736666666666668</v>
+        <v>0.79</v>
       </c>
       <c r="J25">
         <f t="shared" si="6"/>
-        <v>83.40240378104707</v>
+        <v>66.016694702870566</v>
       </c>
       <c r="L25">
-        <v>0.40966666666666668</v>
+        <v>0.57200000000000006</v>
       </c>
       <c r="M25">
         <f t="shared" si="7"/>
-        <v>30.717312992423651</v>
+        <v>47.534639206271258</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>0.5</v>
-      </c>
       <c r="C26">
-        <v>0.91500000000000004</v>
+        <v>0.90699999999999992</v>
       </c>
       <c r="D26">
         <f t="shared" si="4"/>
-        <v>79.889429537086599</v>
+        <v>70.933245325014255</v>
       </c>
       <c r="F26">
-        <v>0.59433333333333327</v>
+        <v>0.44333333333333336</v>
       </c>
       <c r="G26">
         <f t="shared" si="5"/>
-        <v>58.325155381092571</v>
+        <v>35.975124688970709</v>
       </c>
       <c r="I26">
-        <v>0.97333333333333327</v>
+        <v>0.87733333333333341</v>
       </c>
       <c r="J26">
         <f t="shared" si="6"/>
-        <v>75.608512586357463</v>
+        <v>73.314742809263862</v>
       </c>
       <c r="L26">
-        <v>0.18966666666666665</v>
+        <v>0.49</v>
       </c>
       <c r="M26">
         <f t="shared" si="7"/>
-        <v>14.221441084368635</v>
+        <v>40.720232886491104</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
       <c r="C27">
-        <v>0.6156666666666667</v>
+        <v>0.49266666666666675</v>
       </c>
       <c r="D27">
         <f t="shared" si="4"/>
-        <v>53.754381185791964</v>
+        <v>38.52970841248478</v>
       </c>
       <c r="F27">
-        <v>0.41233333333333338</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="G27">
         <f t="shared" si="5"/>
-        <v>40.464507687275116</v>
+        <v>32.458759117868304</v>
       </c>
       <c r="I27">
-        <v>0.44666666666666671</v>
+        <v>0.5073333333333333</v>
       </c>
       <c r="J27">
         <f t="shared" si="6"/>
-        <v>34.697057145794183</v>
+        <v>42.395531366147253</v>
       </c>
       <c r="L27">
-        <v>0.13966666666666669</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="M27">
         <f t="shared" si="7"/>
-        <v>10.47237928708341</v>
+        <v>33.157903921857049</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>3</v>
-      </c>
       <c r="C28">
-        <v>0.27600000000000002</v>
+        <v>0.24133333333333332</v>
       </c>
       <c r="D28">
         <f t="shared" si="4"/>
-        <v>24.097795139055631</v>
+        <v>18.873821982840983</v>
       </c>
       <c r="F28">
-        <v>0.19466666666666665</v>
+        <v>0.23</v>
       </c>
       <c r="G28">
         <f t="shared" si="5"/>
-        <v>19.103696434412822</v>
+        <v>18.663786492774275</v>
       </c>
       <c r="I28">
-        <v>0.16866666666666666</v>
+        <v>0.27866666666666667</v>
       </c>
       <c r="J28">
         <f t="shared" si="6"/>
-        <v>13.102023071471535</v>
+        <v>23.286901591392319</v>
       </c>
       <c r="L28">
-        <v>0.12466666666666666</v>
+        <v>0.27499999999999997</v>
       </c>
       <c r="M28">
         <f t="shared" si="7"/>
-        <v>9.3476607478978391</v>
+        <v>22.853191926091942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>